<commit_message>
Se modificó como calcular los días no operativos
</commit_message>
<xml_diff>
--- a/equipos_costanera.xlsx
+++ b/equipos_costanera.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/camilo/Desktop/PROYECTOS/ROTACION/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA9544F1-5AD1-F547-939F-A0E4FB5D47B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7A0992F-B4FB-8E47-A418-2A7EDAFE5A82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -556,7 +556,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="18.5" customWidth="1"/>
+    <col min="2" max="2" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27.33203125" customWidth="1"/>
     <col min="8" max="8" width="33.6640625" customWidth="1"/>
     <col min="9" max="9" width="27" customWidth="1"/>

</xml_diff>